<commit_message>
actualización 2 _ 1
</commit_message>
<xml_diff>
--- a/tipo_cambio_tasas_interes.xlsx
+++ b/tipo_cambio_tasas_interes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A9B3DD-1147-4B0C-8305-E47E78595CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0597D8-7437-4524-9595-ED568515DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -703,7 +703,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -723,9 +723,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -957,8 +955,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E7" totalsRowShown="0" dataDxfId="28" dataCellStyle="Moneda">
-  <autoFilter ref="A1:E7" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E8" totalsRowShown="0" dataDxfId="28" dataCellStyle="Moneda">
+  <autoFilter ref="A1:E8" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
     <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="27"/>
@@ -971,8 +969,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F8" totalsRowShown="0" dataDxfId="23">
-  <autoFilter ref="A1:F8" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F9" totalsRowShown="0" dataDxfId="23">
+  <autoFilter ref="A1:F9" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
     <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="22"/>
@@ -986,8 +984,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}" name="Tabla24" displayName="Tabla24" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}" name="Tabla24" displayName="Tabla24" ref="A1:F9" totalsRowShown="0">
+  <autoFilter ref="A1:F9" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2E0B3A81-10BF-4919-93D3-DFCB7943009F}" name="Año"/>
     <tableColumn id="2" xr3:uid="{4DDFFDA1-F291-46D8-8D65-F7040EF322C5}" name="Fecha" dataDxfId="17"/>
@@ -1023,8 +1021,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H7" totalsRowShown="0">
-  <autoFilter ref="A1:H7" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7676C863-947F-4296-8B2C-4C1C2493E9D9}" name="Año"/>
     <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="3"/>
@@ -1342,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1458,10 +1456,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="15">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
         <v>45967</v>
       </c>
       <c r="C7" s="2">
@@ -1472,6 +1470,23 @@
       </c>
       <c r="E7" s="2">
         <v>18.553000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45968</v>
+      </c>
+      <c r="C8" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>18.529</v>
+      </c>
+      <c r="E8" s="2">
+        <v>18.446999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1487,7 +1502,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:F8"/>
+      <selection activeCell="A9" sqref="A9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1638,10 +1653,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
-        <v>2025</v>
-      </c>
-      <c r="B8" s="17">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
         <v>45968</v>
       </c>
       <c r="C8" s="3">
@@ -1658,6 +1673,24 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45971</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.51E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7.6200000000000004E-2</v>
+      </c>
       <c r="G9" s="9"/>
     </row>
   </sheetData>
@@ -1670,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4FBFFC-676F-4493-85F5-BF4178BC747B}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" activeCellId="1" sqref="A7:F7 A8:F8"/>
+      <selection activeCell="A9" sqref="A9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1804,10 +1837,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="17">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
         <v>45968</v>
       </c>
       <c r="C7" s="3">
@@ -1824,10 +1857,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
-        <v>2025</v>
-      </c>
-      <c r="B8" s="17">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
         <v>45968</v>
       </c>
       <c r="C8" s="3">
@@ -1841,6 +1874,26 @@
       </c>
       <c r="F8" s="3">
         <v>7.8799999999999995E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45971</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.51E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7.6200000000000004E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1853,10 +1906,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B7A3E5-7422-42F6-B226-5BFEA691299B}">
-  <dimension ref="A1:N7"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2132,10 +2188,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="17">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
         <v>45967</v>
       </c>
       <c r="C7" s="5">
@@ -2173,6 +2229,47 @@
       </c>
       <c r="N7" s="5">
         <v>4.6900000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="17">
+        <v>45968</v>
+      </c>
+      <c r="C8" s="15">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>3.7599999999999995E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3.5699999999999996E-2</v>
+      </c>
+      <c r="J8" s="5">
+        <v>3.6699999999999997E-2</v>
+      </c>
+      <c r="K8" s="5">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="L8" s="5">
+        <v>4.1100000000000005E-2</v>
+      </c>
+      <c r="M8" s="5">
+        <v>4.6799999999999994E-2</v>
+      </c>
+      <c r="N8" s="5">
+        <v>4.7E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2185,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6F7ED1-F67A-4D3F-B065-CA644B535717}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2368,19 +2465,19 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="19">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
         <v>45967</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7">
         <v>46912.30078125</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7">
         <v>6720.31982421875</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7">
         <v>23053.9921875</v>
       </c>
       <c r="F7" s="5">
@@ -2394,6 +2491,35 @@
       <c r="H7" s="5">
         <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E6)/E6,"")</f>
         <v>-1.8970576208437971E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45968</v>
+      </c>
+      <c r="C8" s="16">
+        <v>46987.1015625</v>
+      </c>
+      <c r="D8" s="16">
+        <v>6728.7998046875</v>
+      </c>
+      <c r="E8" s="16">
+        <v>23004.5390625</v>
+      </c>
+      <c r="F8" s="5">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C7)/C7,"")</f>
+        <v>1.5944811915917908E-3</v>
+      </c>
+      <c r="G8" s="5">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D7)/D7,"")</f>
+        <v>1.2618418007711134E-3</v>
+      </c>
+      <c r="H8" s="5">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E7)/E7,"")</f>
+        <v>-2.1451002758131302E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2583,7 +2709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB728CC-3545-439B-8305-CE331A9F0964}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
integrar RAG de Langchain al chatbot
</commit_message>
<xml_diff>
--- a/tipo_cambio_tasas_interes.xlsx
+++ b/tipo_cambio_tasas_interes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7839ED2D-FFB0-4EF8-A9BF-5C7E1303C4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D9FF9E-3402-45B3-89EB-F56222AB323A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -722,12 +722,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -959,8 +959,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E11" totalsRowShown="0" dataDxfId="28" dataCellStyle="Moneda">
-  <autoFilter ref="A1:E11" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E12" totalsRowShown="0" dataDxfId="28" dataCellStyle="Moneda">
+  <autoFilter ref="A1:E12" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
     <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="27"/>
@@ -973,8 +973,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F12" totalsRowShown="0" dataDxfId="23">
-  <autoFilter ref="A1:F12" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F13" totalsRowShown="0" dataDxfId="23">
+  <autoFilter ref="A1:F13" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
     <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="22"/>
@@ -988,8 +988,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}" name="Tabla24" displayName="Tabla24" ref="A1:F12" totalsRowShown="0">
-  <autoFilter ref="A1:F12" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}" name="Tabla24" displayName="Tabla24" ref="A1:F13" totalsRowShown="0">
+  <autoFilter ref="A1:F13" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2E0B3A81-10BF-4919-93D3-DFCB7943009F}" name="Año"/>
     <tableColumn id="2" xr3:uid="{4DDFFDA1-F291-46D8-8D65-F7040EF322C5}" name="Fecha" dataDxfId="17"/>
@@ -1025,8 +1025,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H11" totalsRowShown="0">
-  <autoFilter ref="A1:H11" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H12" totalsRowShown="0">
+  <autoFilter ref="A1:H12" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7676C863-947F-4296-8B2C-4C1C2493E9D9}" name="Año"/>
     <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="3"/>
@@ -1344,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1528,10 +1528,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
-        <v>2025</v>
-      </c>
-      <c r="B11" s="18">
+      <c r="A11">
+        <v>2025</v>
+      </c>
+      <c r="B11" s="1">
         <v>45973</v>
       </c>
       <c r="C11" s="2">
@@ -1542,6 +1542,23 @@
       </c>
       <c r="E11" s="2">
         <v>18.292999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="14">
+        <v>45974</v>
+      </c>
+      <c r="C12" s="2">
+        <v>18.2805</v>
+      </c>
+      <c r="D12" s="2">
+        <v>18.338999999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>18.257999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1554,9 +1571,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FE10B-CC5B-4887-BA9F-8638E71CB003}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1790,7 +1809,7 @@
       <c r="A12">
         <v>2025</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="1">
         <v>45974</v>
       </c>
       <c r="C12" s="3">
@@ -1803,6 +1822,26 @@
         <v>7.5700000000000003E-2</v>
       </c>
       <c r="F12" s="3">
+        <v>7.6300000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <v>2025</v>
+      </c>
+      <c r="B13" s="18">
+        <v>45975</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="F13" s="3">
         <v>7.6300000000000007E-2</v>
       </c>
     </row>
@@ -1816,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4FBFFC-676F-4493-85F5-BF4178BC747B}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,11 +2088,11 @@
         <v>7.6200000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>2025</v>
-      </c>
-      <c r="B12" s="15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="1">
         <v>45974</v>
       </c>
       <c r="C12" s="3">
@@ -2066,6 +2105,26 @@
         <v>7.5700000000000003E-2</v>
       </c>
       <c r="F12" s="3">
+        <v>7.6300000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <v>2025</v>
+      </c>
+      <c r="B13" s="18">
+        <v>45975</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="F13" s="3">
         <v>7.6300000000000007E-2</v>
       </c>
     </row>
@@ -2082,10 +2141,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2487,10 +2546,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="19">
+      <c r="B10" s="1">
         <v>45973</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="4">
         <v>3.9800000000000002E-2</v>
       </c>
       <c r="D10" s="5">
@@ -2527,6 +2586,56 @@
         <v>4.6699999999999998E-2</v>
       </c>
       <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="18">
+        <v>45974</v>
+      </c>
+      <c r="D11" s="5">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>3.9599999999999996E-2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="I11" s="5">
+        <v>3.5699999999999996E-2</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="K11" s="5">
+        <v>3.8900000000000004E-2</v>
+      </c>
+      <c r="L11" s="5">
+        <v>4.1100000000000005E-2</v>
+      </c>
+      <c r="M11" s="5">
+        <v>4.6900000000000004E-2</v>
+      </c>
+      <c r="N11" s="5">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2538,10 +2647,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6F7ED1-F67A-4D3F-B065-CA644B535717}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2837,19 +2946,19 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
-        <v>2025</v>
-      </c>
-      <c r="B11" s="21">
+      <c r="A11">
+        <v>2025</v>
+      </c>
+      <c r="B11" s="1">
         <v>45973</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11">
         <v>48254.8203125</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11">
         <v>6850.919921875</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11">
         <v>23406.4609375</v>
       </c>
       <c r="F11" s="5">
@@ -2863,6 +2972,35 @@
       <c r="H11" s="5">
         <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E10)/E10,"")</f>
         <v>-2.6350371220487741E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="16">
+        <v>45974</v>
+      </c>
+      <c r="C12" s="15">
+        <v>47457.21875</v>
+      </c>
+      <c r="D12" s="15">
+        <v>6737.490234375</v>
+      </c>
+      <c r="E12" s="15">
+        <v>22870.35546875</v>
+      </c>
+      <c r="F12" s="5">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C11)/C11,"")</f>
+        <v>-1.6528951042293863E-2</v>
+      </c>
+      <c r="G12" s="5">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D11)/D11,"")</f>
+        <v>-1.6556854961597027E-2</v>
+      </c>
+      <c r="H12" s="5">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E11)/E11,"")</f>
+        <v>-2.2904166083950513E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2965,10 +3103,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3043,6 +3181,20 @@
         <v>4.2799999999999998E-2</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45931</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4.2799999999999998E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3050,10 +3202,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB728CC-3545-439B-8305-CE331A9F0964}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3194,6 +3346,23 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="20">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="21">
+        <v>45973</v>
+      </c>
+      <c r="C9" s="19">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="19">
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>